<commit_message>
testcase03 login with invalid data
</commit_message>
<xml_diff>
--- a/testData/Data.xlsx
+++ b/testData/Data.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27531"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/99e3a136bf065488/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Renuka\eclipse-workspace\acmedemo\testData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="48" documentId="11_F25DC773A252ABDACC10481AF95962145ADE58E5" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A328D6CC-AEC5-4994-A543-7E1197EE3AD3}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4B664BB-FD05-4A3B-A402-08E33E04A91C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="TC001" sheetId="2" r:id="rId2"/>
+    <sheet name="TC001" sheetId="2" r:id="rId1"/>
+    <sheet name="TC002" sheetId="1" r:id="rId2"/>
+    <sheet name="TC003" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="40">
   <si>
     <t>TestCase ID</t>
   </si>
@@ -128,6 +129,24 @@
   </si>
   <si>
     <t>Rohini</t>
+  </si>
+  <si>
+    <t>TC_003</t>
+  </si>
+  <si>
+    <t>Raj</t>
+  </si>
+  <si>
+    <t>Raj@gmail.com</t>
+  </si>
+  <si>
+    <t>Password@123</t>
+  </si>
+  <si>
+    <t>Expected Result</t>
+  </si>
+  <si>
+    <t>Your email or password is incorrect!</t>
   </si>
 </sst>
 </file>
@@ -173,7 +192,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -196,17 +215,29 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -223,10 +254,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -491,69 +518,6 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D3"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:D1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A1" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-  </sheetData>
-  <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1" xr:uid="{FC00DB3B-B4BC-41A2-9058-0FB9538F0C01}"/>
-    <hyperlink ref="C3" r:id="rId2" xr:uid="{8D60FDCC-07A2-4F74-BCCE-475EC29772B1}"/>
-    <hyperlink ref="D2" r:id="rId3" xr:uid="{5AD0F2CC-D35A-42FD-9212-9872DF961ABE}"/>
-    <hyperlink ref="D3" r:id="rId4" xr:uid="{E8E16EC1-09B6-4928-8AA8-A249D6C1E811}"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B45E7548-9026-4469-B0CA-387337DDDA0B}">
   <dimension ref="A1:P2"/>
   <sheetViews>
@@ -675,4 +639,120 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:D3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K11" sqref="K11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C2" r:id="rId1" xr:uid="{FC00DB3B-B4BC-41A2-9058-0FB9538F0C01}"/>
+    <hyperlink ref="C3" r:id="rId2" xr:uid="{8D60FDCC-07A2-4F74-BCCE-475EC29772B1}"/>
+    <hyperlink ref="D2" r:id="rId3" xr:uid="{5AD0F2CC-D35A-42FD-9212-9872DF961ABE}"/>
+    <hyperlink ref="D3" r:id="rId4" xr:uid="{E8E16EC1-09B6-4928-8AA8-A249D6C1E811}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8061566C-3B4A-4221-8462-26D149CF5ADC}">
+  <dimension ref="A1:E2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="E2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C2" r:id="rId1" xr:uid="{A85F7D36-AA40-451D-AB15-166107C13763}"/>
+    <hyperlink ref="D2" r:id="rId2" xr:uid="{27C41964-F9E6-49FF-8FBC-DE95C443EAE6}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>